<commit_message>
remove redundant units and update test results
</commit_message>
<xml_diff>
--- a/exposan/bsm1/data/initial_conditions.xlsx
+++ b/exposan/bsm1/data/initial_conditions.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\bsm1\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20BE4F37-FAA4-4655-903F-407948734BC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC2BF22-29A8-4CB1-969D-7683232A864D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-13905" yWindow="2085" windowWidth="11580" windowHeight="9150" xr2:uid="{32702723-0D76-4F6C-A6A7-E56FCE88CE75}"/>
+    <workbookView xWindow="-28065" yWindow="735" windowWidth="18240" windowHeight="12225" xr2:uid="{32702723-0D76-4F6C-A6A7-E56FCE88CE75}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="5" r:id="rId1"/>
-    <sheet name="t=0" sheetId="1" r:id="rId2"/>
-    <sheet name="t=1" sheetId="2" r:id="rId3"/>
-    <sheet name="t=5" sheetId="3" r:id="rId4"/>
-    <sheet name="t=10" sheetId="4" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
+    <sheet name="t=0" sheetId="1" r:id="rId3"/>
+    <sheet name="t=1" sheetId="2" r:id="rId4"/>
+    <sheet name="t=5" sheetId="3" r:id="rId5"/>
+    <sheet name="t=10" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
   <si>
     <t>A1</t>
   </si>
@@ -144,7 +145,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -508,12 +519,12 @@
   <dimension ref="A1:N9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -554,7 +565,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -598,7 +609,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -642,7 +653,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -686,7 +697,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -730,7 +741,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -738,44 +749,408 @@
         <v>30</v>
       </c>
       <c r="C6">
-        <v>0.88949</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>1149.1251999999999</v>
+        <v>1000</v>
       </c>
       <c r="E6">
-        <v>49.305599999999998</v>
+        <v>100</v>
       </c>
       <c r="F6">
-        <v>2559.3436000000002</v>
+        <v>500</v>
       </c>
       <c r="G6">
-        <v>149.7971</v>
+        <v>100</v>
       </c>
       <c r="H6">
-        <v>452.21109999999999</v>
+        <v>100</v>
       </c>
       <c r="I6">
-        <v>0.49093999999999999</v>
+        <v>2</v>
       </c>
       <c r="J6">
-        <v>10.4152</v>
+        <v>20</v>
       </c>
       <c r="K6">
-        <v>1.7333000000000001</v>
+        <v>2</v>
       </c>
       <c r="L6">
-        <v>0.68828</v>
+        <v>1</v>
       </c>
       <c r="M6">
-        <v>3.5272000000000001</v>
+        <v>1</v>
       </c>
       <c r="N6">
-        <f>4.1256*12</f>
-        <v>49.507200000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>30</v>
+      </c>
+      <c r="C7">
+        <v>5</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>20</v>
+      </c>
+      <c r="K7">
+        <v>2</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>1000</v>
+      </c>
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8">
+        <v>500</v>
+      </c>
+      <c r="G8">
+        <v>100</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>20</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <v>70</v>
+      </c>
+      <c r="F9">
+        <v>200</v>
+      </c>
+      <c r="G9">
+        <v>300</v>
+      </c>
+      <c r="H9">
+        <v>350</v>
+      </c>
+      <c r="I9">
+        <v>350</v>
+      </c>
+      <c r="J9">
+        <v>2000</v>
+      </c>
+      <c r="K9">
+        <v>4000</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="B1:N1">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9AFB19-985F-4A74-914B-496332EAA538}">
+  <dimension ref="A1:N9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>500</v>
+      </c>
+      <c r="G2">
+        <v>100</v>
+      </c>
+      <c r="H2">
+        <v>100</v>
+      </c>
+      <c r="I2">
+        <v>2</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>2</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>100</v>
+      </c>
+      <c r="F3">
+        <v>500</v>
+      </c>
+      <c r="G3">
+        <v>100</v>
+      </c>
+      <c r="H3">
+        <v>100</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>20</v>
+      </c>
+      <c r="K3">
+        <v>2</v>
+      </c>
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4">
+        <v>500</v>
+      </c>
+      <c r="G4">
+        <v>100</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>20</v>
+      </c>
+      <c r="K4">
+        <v>2</v>
+      </c>
+      <c r="L4">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>1000</v>
+      </c>
+      <c r="E5">
+        <v>100</v>
+      </c>
+      <c r="F5">
+        <v>500</v>
+      </c>
+      <c r="G5">
+        <v>100</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5">
+        <v>2</v>
+      </c>
+      <c r="J5">
+        <v>20</v>
+      </c>
+      <c r="K5">
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <v>1000</v>
+      </c>
+      <c r="E6">
+        <v>100</v>
+      </c>
+      <c r="F6">
+        <v>500</v>
+      </c>
+      <c r="G6">
+        <v>100</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6">
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <v>20</v>
+      </c>
+      <c r="K6">
+        <v>2</v>
+      </c>
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -802,7 +1177,7 @@
         <v>49.507200000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -825,7 +1200,7 @@
         <v>2.3261380370000002</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -870,7 +1245,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540DF28A-4570-4622-9A8A-5FE85A0B28FC}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -878,9 +1253,9 @@
       <selection sqref="A1:N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -921,7 +1296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -965,7 +1340,7 @@
         <v>31.656621959696764</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1009,7 +1384,7 @@
         <v>13.071031765881841</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1053,7 +1428,7 @@
         <v>41.8376580983292</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1097,7 +1472,7 @@
         <v>7.6375751887198078</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1141,7 +1516,7 @@
         <v>3.0525875853357602</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1167,7 +1542,7 @@
         <v>49.507200000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1190,7 +1565,7 @@
         <v>4.89664130704932</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1235,7 +1610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB01DA0-85A6-433D-BA61-05716F44C1B2}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -1243,9 +1618,9 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1286,7 +1661,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1705,7 @@
         <v>56.079439503903963</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1374,7 +1749,7 @@
         <v>57.354810651790913</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1418,7 +1793,7 @@
         <v>53.877447863534876</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1462,7 +1837,7 @@
         <v>50.427541936951087</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1506,7 +1881,7 @@
         <v>47.715265238126044</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1532,7 +1907,7 @@
         <v>46.414747749390486</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1555,7 +1930,7 @@
         <v>4.4742864742827102</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1600,7 +1975,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D26E38B-54CD-4D1B-B51F-E4BB6067FBAE}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -1608,9 +1983,9 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1651,7 +2026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1695,7 +2070,7 @@
         <v>62.509964925265919</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1739,7 +2114,7 @@
         <v>64.107219875887068</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1783,7 +2158,7 @@
         <v>60.484556316927005</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1827,7 +2202,7 @@
         <v>56.817714709040999</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1871,7 +2246,7 @@
         <v>54.356174470380125</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1897,7 +2272,7 @@
         <v>54.324619836396963</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1920,7 +2295,7 @@
         <v>5.5920824737116304</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1965,7 +2340,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24FFA4D-809F-4F7C-A10C-2A24CD6388A4}">
   <dimension ref="A1:N9"/>
   <sheetViews>
@@ -1973,9 +2348,9 @@
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2016,7 +2391,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2060,7 +2435,7 @@
         <v>62.015909339771525</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2104,7 +2479,7 @@
         <v>63.734365340730719</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2148,7 +2523,7 @@
         <v>59.663430267968522</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2192,7 +2567,7 @@
         <v>55.577371832611078</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2236,7 +2611,7 @@
         <v>53.319931318453072</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2262,7 +2637,7 @@
         <v>53.376844875010555</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2285,7 +2660,7 @@
         <v>6.4246344079408404</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
add ASM validation modules
</commit_message>
<xml_diff>
--- a/exposan/bsm1/data/initial_conditions.xlsx
+++ b/exposan/bsm1/data/initial_conditions.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joy_c\Dropbox\PhD\Research\QSD\codes_developing\EXPOsan\exposan\bsm1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Library/CloudStorage/OneDrive-Personal/Coding/es/exposan/bsm1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FC2BF22-29A8-4CB1-969D-7683232A864D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{737315FD-CD60-874E-8BDD-1BEFFDF7621E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28065" yWindow="735" windowWidth="18240" windowHeight="12225" xr2:uid="{32702723-0D76-4F6C-A6A7-E56FCE88CE75}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{32702723-0D76-4F6C-A6A7-E56FCE88CE75}"/>
   </bookViews>
   <sheets>
     <sheet name="default" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId2"/>
-    <sheet name="t=0" sheetId="1" r:id="rId3"/>
-    <sheet name="t=1" sheetId="2" r:id="rId4"/>
-    <sheet name="t=5" sheetId="3" r:id="rId5"/>
-    <sheet name="t=10" sheetId="4" r:id="rId6"/>
+    <sheet name="t=0" sheetId="1" r:id="rId2"/>
+    <sheet name="t=1" sheetId="2" r:id="rId3"/>
+    <sheet name="t=5" sheetId="3" r:id="rId4"/>
+    <sheet name="t=10" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="21">
   <si>
     <t>A1</t>
   </si>
@@ -145,17 +144,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -518,13 +507,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9E1BA80-9E8D-4883-B1AD-23C2415115BA}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -565,7 +554,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -609,7 +598,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -653,7 +642,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -697,7 +686,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -741,7 +730,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -785,7 +774,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -811,7 +800,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -834,7 +823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -867,372 +856,6 @@
       </c>
       <c r="K9">
         <v>4000</v>
-      </c>
-    </row>
-  </sheetData>
-  <conditionalFormatting sqref="B1:N1">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="lessThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F9AFB19-985F-4A74-914B-496332EAA538}">
-  <dimension ref="A1:N9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>1000</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <v>500</v>
-      </c>
-      <c r="G2">
-        <v>100</v>
-      </c>
-      <c r="H2">
-        <v>100</v>
-      </c>
-      <c r="I2">
-        <v>2</v>
-      </c>
-      <c r="J2">
-        <v>20</v>
-      </c>
-      <c r="K2">
-        <v>2</v>
-      </c>
-      <c r="L2">
-        <v>1</v>
-      </c>
-      <c r="M2">
-        <v>1</v>
-      </c>
-      <c r="N2">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <v>500</v>
-      </c>
-      <c r="G3">
-        <v>100</v>
-      </c>
-      <c r="H3">
-        <v>100</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="J3">
-        <v>20</v>
-      </c>
-      <c r="K3">
-        <v>2</v>
-      </c>
-      <c r="L3">
-        <v>1</v>
-      </c>
-      <c r="M3">
-        <v>1</v>
-      </c>
-      <c r="N3">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-      <c r="D4">
-        <v>1000</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <v>500</v>
-      </c>
-      <c r="G4">
-        <v>100</v>
-      </c>
-      <c r="H4">
-        <v>100</v>
-      </c>
-      <c r="I4">
-        <v>2</v>
-      </c>
-      <c r="J4">
-        <v>20</v>
-      </c>
-      <c r="K4">
-        <v>2</v>
-      </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
-      <c r="N4">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
-      <c r="C5">
-        <v>5</v>
-      </c>
-      <c r="D5">
-        <v>1000</v>
-      </c>
-      <c r="E5">
-        <v>100</v>
-      </c>
-      <c r="F5">
-        <v>500</v>
-      </c>
-      <c r="G5">
-        <v>100</v>
-      </c>
-      <c r="H5">
-        <v>100</v>
-      </c>
-      <c r="I5">
-        <v>2</v>
-      </c>
-      <c r="J5">
-        <v>20</v>
-      </c>
-      <c r="K5">
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-      <c r="N5">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6">
-        <v>5</v>
-      </c>
-      <c r="D6">
-        <v>1000</v>
-      </c>
-      <c r="E6">
-        <v>100</v>
-      </c>
-      <c r="F6">
-        <v>500</v>
-      </c>
-      <c r="G6">
-        <v>100</v>
-      </c>
-      <c r="H6">
-        <v>100</v>
-      </c>
-      <c r="I6">
-        <v>2</v>
-      </c>
-      <c r="J6">
-        <v>20</v>
-      </c>
-      <c r="K6">
-        <v>2</v>
-      </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-      <c r="N6">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7">
-        <v>0.88949</v>
-      </c>
-      <c r="I7">
-        <v>0.49093999999999999</v>
-      </c>
-      <c r="J7">
-        <v>10.4152</v>
-      </c>
-      <c r="K7">
-        <v>1.7333000000000001</v>
-      </c>
-      <c r="L7">
-        <v>0.68828</v>
-      </c>
-      <c r="N7">
-        <f>4.1256*12</f>
-        <v>49.507200000000005</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>1507.8928249999999</v>
-      </c>
-      <c r="E8">
-        <v>89.394451200000006</v>
-      </c>
-      <c r="F8">
-        <v>5913.5546210000002</v>
-      </c>
-      <c r="G8">
-        <v>372.68631090000002</v>
-      </c>
-      <c r="H8">
-        <v>641.78432469999996</v>
-      </c>
-      <c r="M8">
-        <v>2.3261380370000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>12.4969</v>
-      </c>
-      <c r="C9">
-        <v>18.113199999999999</v>
-      </c>
-      <c r="D9">
-        <v>29.540199999999999</v>
-      </c>
-      <c r="E9">
-        <v>68.978099999999998</v>
-      </c>
-      <c r="F9">
-        <v>356.07470000000001</v>
-      </c>
-      <c r="G9">
-        <v>356.07470000000001</v>
-      </c>
-      <c r="H9">
-        <v>356.07470000000001</v>
-      </c>
-      <c r="I9">
-        <v>356.07470000000001</v>
-      </c>
-      <c r="J9">
-        <v>356.07470000000001</v>
-      </c>
-      <c r="K9">
-        <v>6393.9844000000003</v>
       </c>
     </row>
   </sheetData>
@@ -1245,17 +868,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540DF28A-4570-4622-9A8A-5FE85A0B28FC}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection sqref="A1:N9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1296,7 +919,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +963,7 @@
         <v>31.656621959696764</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1384,7 +1007,7 @@
         <v>13.071031765881841</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1428,7 +1051,7 @@
         <v>41.8376580983292</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1472,7 +1095,7 @@
         <v>7.6375751887198078</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1516,7 +1139,7 @@
         <v>3.0525875853357602</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1542,7 +1165,7 @@
         <v>49.507200000000005</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1565,7 +1188,7 @@
         <v>4.89664130704932</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1610,17 +1233,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BB01DA0-85A6-433D-BA61-05716F44C1B2}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -1661,7 +1284,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1705,7 +1328,7 @@
         <v>56.079439503903963</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -1749,7 +1372,7 @@
         <v>57.354810651790913</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1793,7 +1416,7 @@
         <v>53.877447863534876</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1837,7 +1460,7 @@
         <v>50.427541936951087</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1881,7 +1504,7 @@
         <v>47.715265238126044</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1907,7 +1530,7 @@
         <v>46.414747749390486</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1930,7 +1553,7 @@
         <v>4.4742864742827102</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1975,17 +1598,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D26E38B-54CD-4D1B-B51F-E4BB6067FBAE}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2026,7 +1649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2070,7 +1693,7 @@
         <v>62.509964925265919</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2114,7 +1737,7 @@
         <v>64.107219875887068</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2158,7 +1781,7 @@
         <v>60.484556316927005</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2202,7 +1825,7 @@
         <v>56.817714709040999</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2246,7 +1869,7 @@
         <v>54.356174470380125</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2272,7 +1895,7 @@
         <v>54.324619836396963</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2295,7 +1918,7 @@
         <v>5.5920824737116304</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2340,17 +1963,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D24FFA4D-809F-4F7C-A10C-2A24CD6388A4}">
   <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>8</v>
       </c>
@@ -2391,7 +2014,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2435,7 +2058,7 @@
         <v>62.015909339771525</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2479,7 +2102,7 @@
         <v>63.734365340730719</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2523,7 +2146,7 @@
         <v>59.663430267968522</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2567,7 +2190,7 @@
         <v>55.577371832611078</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2611,7 +2234,7 @@
         <v>53.319931318453072</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2637,7 +2260,7 @@
         <v>53.376844875010555</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2660,7 +2283,7 @@
         <v>6.4246344079408404</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>

</xml_diff>